<commit_message>
Update version 9 untuk sidang akhir
</commit_message>
<xml_diff>
--- a/Data/ManualPerhitungan/Beberapa Percobaan.xlsx
+++ b/Data/ManualPerhitungan/Beberapa Percobaan.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\RekomendasiBeasiswa\Data\ManualPerhitungan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A55A3715-A3A2-44B8-9C1E-AF8181F30BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A699EE-883D-435C-86AD-7F8B1AA04337}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E5EF371-02DB-4F07-B227-B044743477B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5E5EF371-02DB-4F07-B227-B044743477B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
   <si>
     <t>Tanpa REP</t>
   </si>
@@ -76,13 +77,49 @@
   </si>
   <si>
     <t>Rata-Rata</t>
+  </si>
+  <si>
+    <t>Percobaan ke-</t>
+  </si>
+  <si>
+    <t>Tanpa Penghapusan Outlier</t>
+  </si>
+  <si>
+    <t>10 Percobaan Pada Pembentukan Decision Tree</t>
+  </si>
+  <si>
+    <t>Percobaan ke</t>
+  </si>
+  <si>
+    <t>Jumlah Node</t>
+  </si>
+  <si>
+    <t>Kedalaman (Level)</t>
+  </si>
+  <si>
+    <t>Tertinggi</t>
+  </si>
+  <si>
+    <t>Terkecil</t>
+  </si>
+  <si>
+    <t>Jumlah Data</t>
+  </si>
+  <si>
+    <t>Iya</t>
+  </si>
+  <si>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>Data Training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,16 +141,43 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -147,23 +211,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -173,6 +280,41 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACBF068-43ED-42BD-9785-65CD29909FE5}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,39 +643,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
       <c r="V1" t="s">
         <v>12</v>
       </c>
@@ -542,70 +684,70 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
+      <c r="S2" s="6"/>
+      <c r="T2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1" t="s">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1" t="s">
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1" t="s">
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="1"/>
+      <c r="AC2" s="6"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -691,16 +833,16 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>0.62</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>0.69</v>
       </c>
       <c r="D4">
         <v>0.52</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>0.59</v>
       </c>
       <c r="F4">
@@ -709,10 +851,10 @@
       <c r="G4">
         <v>0.69</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="1">
         <v>0.7</v>
       </c>
       <c r="L4">
@@ -733,16 +875,16 @@
       <c r="U4">
         <v>0.64</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4" s="1">
         <v>0.79</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="1">
         <v>0.82</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4" s="1">
         <v>0.76</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AC4" s="1">
         <v>0.89</v>
       </c>
     </row>
@@ -750,10 +892,10 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="2">
         <v>0.38</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <f>1-C4</f>
         <v>0.31000000000000005</v>
       </c>
@@ -866,43 +1008,49 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:29" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>0</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="A10" s="4">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4">
         <v>0.66666700000000001</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>0.69696999999999998</v>
       </c>
       <c r="D10">
         <f>C10-B10</f>
         <v>3.0302999999999969E-2</v>
       </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
         <v>0.57777800000000001</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <v>0.6</v>
       </c>
       <c r="H10">
@@ -911,26 +1059,26 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4">
         <v>0.66666700000000001</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>0.69696999999999998</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D31" si="13">C11-B11</f>
         <v>3.0302999999999969E-2</v>
       </c>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
         <v>0.6</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>0.6</v>
       </c>
       <c r="H11">
@@ -939,26 +1087,26 @@
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="4">
         <v>0.57575799999999999</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>0.54545500000000002</v>
       </c>
       <c r="D12">
         <f t="shared" si="13"/>
         <v>-3.0302999999999969E-2</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>2</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="4">
         <v>0.44444400000000001</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>0.42222199999999999</v>
       </c>
       <c r="H12">
@@ -967,26 +1115,26 @@
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="4">
         <v>0.51515200000000005</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <v>0.60606099999999996</v>
       </c>
       <c r="D13">
         <f t="shared" si="13"/>
         <v>9.0908999999999907E-2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="4">
         <v>0.466667</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <v>0.51111099999999998</v>
       </c>
       <c r="H13">
@@ -995,26 +1143,26 @@
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="4">
         <v>0.63636400000000004</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>0.63636400000000004</v>
       </c>
       <c r="D14">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>4</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <v>0.68888899999999997</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <v>0.68888899999999997</v>
       </c>
       <c r="H14">
@@ -1023,26 +1171,26 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="4">
         <v>5</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="4">
         <v>0.75757600000000003</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="4">
         <v>0.75757600000000003</v>
       </c>
       <c r="D15">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>5</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <v>0.64444400000000002</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>0.77777799999999997</v>
       </c>
       <c r="H15">
@@ -1051,26 +1199,26 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>0.484848</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>0.51515200000000005</v>
       </c>
       <c r="D16">
         <f t="shared" si="13"/>
         <v>3.0304000000000053E-2</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>6</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="4">
         <v>0.75555600000000001</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <v>0.64444400000000002</v>
       </c>
       <c r="H16">
@@ -1079,26 +1227,26 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>0.57575799999999999</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>0.54545500000000002</v>
       </c>
       <c r="D17">
         <f t="shared" si="13"/>
         <v>-3.0302999999999969E-2</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>7</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>0.55555600000000005</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <v>0.68888899999999997</v>
       </c>
       <c r="H17">
@@ -1107,26 +1255,26 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>0.69696999999999998</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>0.66666700000000001</v>
       </c>
       <c r="D18">
         <f t="shared" si="13"/>
         <v>-3.0302999999999969E-2</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>8</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>0.75555600000000001</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <v>0.75555600000000001</v>
       </c>
       <c r="H18">
@@ -1135,26 +1283,26 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>0.63636400000000004</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>0.60606099999999996</v>
       </c>
       <c r="D19">
         <f t="shared" si="13"/>
         <v>-3.030300000000008E-2</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>9</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <v>0.55555600000000005</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <v>0.55555600000000005</v>
       </c>
       <c r="H19">
@@ -1163,26 +1311,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="4">
         <v>10</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>0.60606099999999996</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>0.45454499999999998</v>
       </c>
       <c r="D20">
         <f t="shared" si="13"/>
         <v>-0.15151599999999998</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>10</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>0.57777800000000001</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <v>0.57777800000000001</v>
       </c>
       <c r="H20">
@@ -1191,26 +1339,26 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="4">
         <v>11</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>0.51515200000000005</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>0.60606099999999996</v>
       </c>
       <c r="D21">
         <f t="shared" si="13"/>
         <v>9.0908999999999907E-2</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>11</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>0.64444400000000002</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <v>0.62222200000000005</v>
       </c>
       <c r="H21">
@@ -1219,26 +1367,26 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="4">
         <v>12</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="4">
         <v>0.60606099999999996</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>0.60606099999999996</v>
       </c>
       <c r="D22">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>12</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="4">
         <v>0.466667</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4">
         <v>0.48888900000000002</v>
       </c>
       <c r="H22">
@@ -1247,26 +1395,26 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="4">
         <v>13</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="4">
         <v>0.60606099999999996</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="4">
         <v>0.63636400000000004</v>
       </c>
       <c r="D23">
         <f t="shared" si="13"/>
         <v>3.030300000000008E-2</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4">
         <v>13</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="4">
         <v>0.68888899999999997</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="4">
         <v>0.66666700000000001</v>
       </c>
       <c r="H23">
@@ -1275,26 +1423,26 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="4">
         <v>14</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="4">
         <v>0.787879</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="4">
         <v>0.72727299999999995</v>
       </c>
       <c r="D24">
         <f t="shared" si="13"/>
         <v>-6.0606000000000049E-2</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="4">
         <v>14</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="4">
         <v>0.55555600000000005</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="4">
         <v>0.57777800000000001</v>
       </c>
       <c r="H24">
@@ -1303,26 +1451,26 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="4">
         <v>15</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="4">
         <v>0.66666700000000001</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="4">
         <v>0.57575799999999999</v>
       </c>
       <c r="D25">
         <f t="shared" si="13"/>
         <v>-9.0909000000000018E-2</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>15</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="4">
         <v>0.66666700000000001</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="4">
         <v>0.62222200000000005</v>
       </c>
       <c r="H25">
@@ -1331,26 +1479,26 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="4">
         <v>16</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="4">
         <v>0.63636400000000004</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="4">
         <v>0.57575799999999999</v>
       </c>
       <c r="D26">
         <f t="shared" si="13"/>
         <v>-6.0606000000000049E-2</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="4">
         <v>16</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="4">
         <v>0.66666700000000001</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="4">
         <v>0.64444400000000002</v>
       </c>
       <c r="H26">
@@ -1359,26 +1507,26 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>17</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="4">
         <v>0.75757600000000003</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>0.75757600000000003</v>
       </c>
       <c r="D27">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="4">
         <v>17</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="4">
         <v>0.73333300000000001</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="4">
         <v>0.73333300000000001</v>
       </c>
       <c r="H27">
@@ -1387,26 +1535,26 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="4">
         <v>18</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>0.60606099999999996</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>0.63636400000000004</v>
       </c>
       <c r="D28">
         <f t="shared" si="13"/>
         <v>3.030300000000008E-2</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>18</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="4">
         <v>0.71111100000000005</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>0.66666700000000001</v>
       </c>
       <c r="H28">
@@ -1415,26 +1563,26 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="4">
         <v>19</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="4">
         <v>0.63636400000000004</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="4">
         <v>0.63636400000000004</v>
       </c>
       <c r="D29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="4">
         <v>19</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="4">
         <v>0.55555600000000005</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="4">
         <v>0.6</v>
       </c>
       <c r="H29">
@@ -1443,26 +1591,26 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="4">
         <v>20</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="4">
         <v>0.69696999999999998</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>0.75757600000000003</v>
       </c>
       <c r="D30">
         <f t="shared" si="13"/>
         <v>6.0606000000000049E-2</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>20</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="4">
         <v>0.62222200000000005</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="4">
         <v>0.62222200000000005</v>
       </c>
       <c r="H30">
@@ -1471,26 +1619,26 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="4">
         <v>21</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="4">
         <v>0.60606099999999996</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="4">
         <v>0.66666700000000001</v>
       </c>
       <c r="D31">
         <f t="shared" si="13"/>
         <v>6.0606000000000049E-2</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="4">
         <v>21</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="4">
         <v>0.62222200000000005</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="4">
         <v>0.62222200000000005</v>
       </c>
       <c r="H31">
@@ -1529,6 +1677,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="R2:S2"/>
@@ -1536,21 +1697,447 @@
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47230B20-51BF-4B1C-A119-44654C4F1D74}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <f>SUM(C4:D4)</f>
+        <v>150</v>
+      </c>
+      <c r="C4" s="13">
+        <v>80</v>
+      </c>
+      <c r="D4" s="13">
+        <v>70</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F4" s="18">
+        <f>1-E4</f>
+        <v>0.42400000000000004</v>
+      </c>
+      <c r="G4" s="13">
+        <v>66</v>
+      </c>
+      <c r="H4" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13">
+        <f t="shared" ref="B5:B13" si="0">SUM(C5:D5)</f>
+        <v>150</v>
+      </c>
+      <c r="C5" s="13">
+        <v>79</v>
+      </c>
+      <c r="D5" s="13">
+        <v>71</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F5" s="18">
+        <f>1-E5</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="G5" s="13">
+        <v>64</v>
+      </c>
+      <c r="H5" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C6" s="13">
+        <v>76</v>
+      </c>
+      <c r="D6" s="13">
+        <v>74</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F6" s="18">
+        <f t="shared" ref="F6:F13" si="1">1-E6</f>
+        <v>0.45499999999999996</v>
+      </c>
+      <c r="G6" s="13">
+        <v>70</v>
+      </c>
+      <c r="H6" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C7" s="13">
+        <v>83</v>
+      </c>
+      <c r="D7" s="13">
+        <v>67</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="1"/>
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="G7" s="13">
+        <v>80</v>
+      </c>
+      <c r="H7" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C8" s="13">
+        <v>81</v>
+      </c>
+      <c r="D8" s="13">
+        <v>69</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="1"/>
+        <v>0.33299999999999996</v>
+      </c>
+      <c r="G8" s="13">
+        <v>68</v>
+      </c>
+      <c r="H8" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C9" s="13">
+        <v>84</v>
+      </c>
+      <c r="D9" s="13">
+        <v>66</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="1"/>
+        <v>0.33299999999999996</v>
+      </c>
+      <c r="G9" s="13">
+        <v>66</v>
+      </c>
+      <c r="H9" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C10" s="13">
+        <v>81</v>
+      </c>
+      <c r="D10" s="13">
+        <v>69</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="1"/>
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G10" s="13">
+        <v>72</v>
+      </c>
+      <c r="H10" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C11" s="13">
+        <v>81</v>
+      </c>
+      <c r="D11" s="13">
+        <v>69</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F11" s="18">
+        <f t="shared" si="1"/>
+        <v>0.42400000000000004</v>
+      </c>
+      <c r="G11" s="13">
+        <v>72</v>
+      </c>
+      <c r="H11" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C12" s="13">
+        <v>75</v>
+      </c>
+      <c r="D12" s="13">
+        <v>75</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="18">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G12" s="13">
+        <v>66</v>
+      </c>
+      <c r="H12" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C13" s="13">
+        <v>80</v>
+      </c>
+      <c r="D13" s="13">
+        <v>70</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" si="1"/>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="G13" s="13">
+        <v>72</v>
+      </c>
+      <c r="H13" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="18">
+        <f>AVERAGE(E4:E13)</f>
+        <v>0.59729999999999994</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" ref="F14:H14" si="2">AVERAGE(F4:F13)</f>
+        <v>0.4027</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="2"/>
+        <v>69.599999999999994</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="2"/>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="18">
+        <f>MAX(E4:E13)</f>
+        <v>0.7</v>
+      </c>
+      <c r="F15" s="18">
+        <f t="shared" ref="F15:H15" si="3">MAX(F4:F13)</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="18">
+        <f>MIN(E4:E13)</f>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F16" s="18">
+        <f t="shared" ref="F16:H16" si="4">MIN(F4:F13)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="H16" s="13">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>